<commit_message>
certification program pdf added
</commit_message>
<xml_diff>
--- a/public/documents/board_members.xlsx
+++ b/public/documents/board_members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\shripal\bmet\public\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://albertahealthservices-my.sharepoint.com/personal/shripal_parikh_albertahealthservices_ca/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4747FB68-009D-4DD5-A845-828981F5F001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{1209C2C7-6693-4E56-B724-DD06D64046BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,28 +25,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Shripal Parikh</t>
-  </si>
-  <si>
-    <t>Christine</t>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Director of Support Services, Eastern Urban Zone</t>
+  </si>
+  <si>
+    <t>Co-Chair Biomedical</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Dialysis Technologist. Alberta Health Services</t>
+  </si>
+  <si>
+    <t>Co-Chair Dialysis</t>
+  </si>
+  <si>
+    <t>Vice-Chair Dialysis</t>
+  </si>
+  <si>
+    <t>Vice-Chair Biomedical</t>
+  </si>
+  <si>
+    <t>Alicia Madore</t>
+  </si>
+  <si>
+    <t>Secretariat</t>
+  </si>
+  <si>
+    <t>Treasurer</t>
+  </si>
+  <si>
+    <t>Anthony Chan</t>
+  </si>
+  <si>
+    <t>Trustee</t>
+  </si>
+  <si>
+    <t>Sarah Deschamps, C.E.T., CBET(c)</t>
+  </si>
+  <si>
+    <t>Murray Greenwood, CET, CBET©</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomedical Engineering Technologist, The University of Ottawa Heart Institute
+</t>
+  </si>
+  <si>
+    <t>Michael Dixon, CBET(c), CHTM</t>
+  </si>
+  <si>
+    <t>Clinical Technology Manager, Mackenzie Health, Sodexo Canada</t>
+  </si>
+  <si>
+    <t>Manager, Biomedical Services, Markham Stouffville Hospital</t>
+  </si>
+  <si>
+    <t>Board member</t>
+  </si>
+  <si>
+    <t>Education Advisor</t>
+  </si>
+  <si>
+    <t>Clinical Engineering Consultant, CHEO, Adjunct Professor, Department of Mechanical Engineering, Faculty of Engineering, University of Ottawa</t>
+  </si>
+  <si>
+    <t>Kim J. Greenwood, MASc., P.Eng, CCE-CA, CET, CBETc FEIC, FCMBES, FACCE</t>
+  </si>
+  <si>
+    <t>Program Head, Biomedical Engineering Technology, BCIT</t>
+  </si>
+  <si>
+    <t>Michael Hopcraft, CBET(c) C.E.T.</t>
+  </si>
+  <si>
+    <t>Imaging Equipment Technologist (MRI), Shared Health Manitoba – Clinical Engineering</t>
+  </si>
+  <si>
+    <t>Christina Cole M.T.M, B.Tech, CHE</t>
+  </si>
+  <si>
+    <t>Aylwin Tagore, cdt</t>
+  </si>
+  <si>
+    <t>Shripal parikh, cdt, CTech</t>
+  </si>
+  <si>
+    <t>Jesse Esperame, C.Tech., CBET(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomedical Technologist, Biomedical Engineering, Victoria General Hospital
+</t>
+  </si>
+  <si>
+    <t>Mr. Joseph Kolodziej, CBET(c), CRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Manager, Canadian Diagnostic Imaging
+</t>
+  </si>
+  <si>
+    <t>David Falagario, CBET(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical Technology Specialist, Insight health tech Planning
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,13 +189,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -351,31 +504,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="124.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>